<commit_message>
Los loops realizados para CWM y FDiver esta incorrectos por lo que se van a repetir los analisis con el paquete FD
</commit_message>
<xml_diff>
--- a/data/raw/response_traits/data_faltante_llena.xlsx
+++ b/data/raw/response_traits/data_faltante_llena.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="253">
   <si>
     <t>familia</t>
   </si>
@@ -1491,7 +1492,7 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1632,6 +1633,19 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1972,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2806,18 +2820,18 @@
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9" s="11" customFormat="1" ht="30">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
       <c r="G40" s="2" t="s">
         <v>159</v>
       </c>
@@ -2848,18 +2862,18 @@
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
       <c r="G42" s="2" t="s">
         <v>171</v>
       </c>
@@ -3275,6 +3289,672 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1">
+      <c r="A2" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="A5" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75">
+      <c r="A13" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="A14" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="23.25" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="55"/>
+      <c r="E26" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D27" s="55"/>
+      <c r="E27" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75">
+      <c r="A35" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75">
+      <c r="A36" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75">
+      <c r="A37" s="48"/>
+      <c r="B37" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75">
+      <c r="A38" s="48"/>
+      <c r="B38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75">
+      <c r="A39" s="48"/>
+      <c r="B39" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75">
+      <c r="A40" s="48"/>
+      <c r="B40" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75">
+      <c r="A41" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75">
+      <c r="A42" s="49"/>
+      <c r="B42" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75">
+      <c r="A43" s="49"/>
+      <c r="B43" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75">
+      <c r="A44" s="49"/>
+      <c r="B44" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75">
+      <c r="A45" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75">
+      <c r="A46" s="50"/>
+      <c r="B46" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75">
+      <c r="A47" s="50"/>
+      <c r="B47" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75">
+      <c r="A48" s="50"/>
+      <c r="B48" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>